<commit_message>
Tablet Size device shows fragment when items clicked.
</commit_message>
<xml_diff>
--- a/Work Sheet.xlsx
+++ b/Work Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Project\Android_Project\MyDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE05AC04-31B4-4D3E-B5BF-4AD9F6E48A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE158D6-53FD-4BA7-A03A-1AF1C759ACD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E594E368-4672-49CF-B70E-1643209E8C9C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Number</t>
   </si>
@@ -217,6 +217,31 @@
   </si>
   <si>
     <t>Setting will have option Font size, Font color, and background Color.</t>
+  </si>
+  <si>
+    <t>Set different Screen Size (Tablet Size)</t>
+  </si>
+  <si>
+    <t>If the device is Tablet, use fragment to show word and meaning
+instead of bottom sheet dialog</t>
+  </si>
+  <si>
+    <t>Create new xml files, adapter, and fragement for tablet size.
+In tablet motitors, clicking word shows Meaning and Part of Speeches
+at Fragment rightside of monitor</t>
+  </si>
+  <si>
+    <t>MainActivity
+BottomSheetDialogAdapter
+FragmentRecyclerViewAdapter
+MainActivityRecyclerViewAdapter
+WordBottomSheetDialog
+MainFragment
+OnItemClick (interface)
+enter_from_right.xml (anim)
+activity_main.xml
+activity_main_fragment_xml
+rv_fragment_pos_mean.xml</t>
   </si>
 </sst>
 </file>
@@ -627,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D84475B-46C5-4C32-807D-CB2AF9B04080}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -742,7 +767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="115.2">
+    <row r="7" spans="1:6" ht="100.8">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -854,6 +879,26 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="187.2">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Option "Setting" functions
</commit_message>
<xml_diff>
--- a/Work Sheet.xlsx
+++ b/Work Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Project\Android_Project\MyDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE158D6-53FD-4BA7-A03A-1AF1C759ACD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69744BA-34F5-4B1B-BFB7-8FCFB131D011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E594E368-4672-49CF-B70E-1643209E8C9C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E594E368-4672-49CF-B70E-1643209E8C9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>User should be able to delete item.</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Create CheckBox to verify which item user wants to delete.
@@ -242,6 +239,18 @@
 activity_main.xml
 activity_main_fragment_xml
 rv_fragment_pos_mean.xml</t>
+  </si>
+  <si>
+    <t>Get Data for "Text Size", "Text Color", and "Background Color" through Dialog,
+then apply the changes to main recyclerview and layout.</t>
+  </si>
+  <si>
+    <t>MainActivity
+MainActivityRecyclerView
+WordsList
+SettingDialog
+activity_main.xml
+dialog_setting.xml</t>
   </si>
 </sst>
 </file>
@@ -654,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D84475B-46C5-4C32-807D-CB2AF9B04080}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -861,24 +870,30 @@
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="100.8">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="187.2">
@@ -886,19 +901,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Keep setting options when restart the application.
</commit_message>
<xml_diff>
--- a/Work Sheet.xlsx
+++ b/Work Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Project\Android_Project\MyDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69744BA-34F5-4B1B-BFB7-8FCFB131D011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5D88A6-5361-4E09-9513-A4B9EA41F850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E594E368-4672-49CF-B70E-1643209E8C9C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E594E368-4672-49CF-B70E-1643209E8C9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Number</t>
   </si>
@@ -251,6 +251,22 @@
 SettingDialog
 activity_main.xml
 dialog_setting.xml</t>
+  </si>
+  <si>
+    <t>Save options in database</t>
+  </si>
+  <si>
+    <t>When the application restarted, save the options and keep them</t>
+  </si>
+  <si>
+    <t>Create new table for options (Text Size, Text Color, and Background Color), 
+then call it on onCreate of Main Activity LifeCycle, and adapt the options.</t>
+  </si>
+  <si>
+    <t>MainActivity
+DBHelper
+AddNewWordDialog
+SettingDialog</t>
   </si>
 </sst>
 </file>
@@ -661,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D84475B-46C5-4C32-807D-CB2AF9B04080}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -916,6 +932,26 @@
         <v>50</v>
       </c>
     </row>
+    <row r="14" spans="1:6" ht="57.6">
+      <c r="A14" s="2">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F2"/>

</xml_diff>